<commit_message>
This was a test for the meeting
Test upload changing news
</commit_message>
<xml_diff>
--- a/docs/content.xlsx
+++ b/docs/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Card Types" sheetId="1" state="hidden" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="381">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -407,6 +407,9 @@
     <t xml:space="preserve">johdy.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">Big News</t>
+  </si>
+  <si>
     <t xml:space="preserve">subtitle</t>
   </si>
   <si>
@@ -1271,7 +1274,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1334,12 +1337,6 @@
       <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1405,7 +1402,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1454,7 +1451,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1462,11 +1459,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1474,12 +1471,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1509,7 +1502,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1676,33 +1669,33 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="25.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="7" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="26.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="7" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="53.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="7" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="7" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>58</v>
@@ -1710,124 +1703,124 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1866,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>40</v>
@@ -1887,7 +1880,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>67</v>
@@ -1931,1194 +1924,1194 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C6" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="n">
         <v>14</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C14" s="7" t="n">
         <v>56</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C19" s="7" t="n">
         <v>146</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C23" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C24" s="7" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C25" s="7" t="n">
         <v>12</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C26" s="7" t="n">
         <v>7</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C29" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C30" s="7" t="n">
         <v>7</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C31" s="7" t="n">
         <v>20</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C33" s="7" t="n">
         <v>6</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C34" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C35" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C38" s="7" t="n">
         <v>3</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C39" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C40" s="7" t="n">
         <v>143</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C41" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C42" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C43" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C44" s="7" t="n">
         <v>10</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C45" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C46" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C47" s="7" t="n">
         <v>32</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C49" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C50" s="7" t="n">
         <v>29</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C51" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C53" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C54" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C55" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C56" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C62" s="7" t="n">
         <v>84</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C64" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C65" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C66" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C68" s="7" t="n">
         <v>33</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C69" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C70" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C72" s="7" t="n">
         <v>4</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C74" s="7" t="n">
         <v>52</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C76" s="7" t="n">
         <v>2</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C77" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3143,19 +3136,19 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="21.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="7" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="7" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3163,15 +3156,15 @@
         <v>78</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F3" s="13"/>
     </row>
@@ -3180,16 +3173,16 @@
         <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F5" s="13"/>
     </row>
@@ -3215,34 +3208,34 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="3" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,66 +3263,64 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="48.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
-        <v>376</v>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>377</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -3354,78 +3345,77 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="30.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
-        <v>376</v>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>376</v>
+      <c r="D3" s="12" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>376</v>
+      <c r="D6" s="12" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -3450,12 +3440,12 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="22.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="3" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,14 +3807,14 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="57.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="7" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="7" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,11 +4384,11 @@
   </sheetPr>
   <dimension ref="G1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G1" s="11" t="s">
@@ -4415,16 +4405,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4447,50 +4437,50 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>58</v>
@@ -4498,33 +4488,33 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="I2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4594,7 +4584,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>40</v>
@@ -4608,7 +4598,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>67</v>
@@ -4656,27 +4646,27 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="7" width="12.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="7" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="7" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>58</v>
@@ -4684,97 +4674,97 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4829,7 +4819,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>40</v>
@@ -4843,7 +4833,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>67</v>
@@ -4854,7 +4844,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>40</v>
@@ -4865,7 +4855,7 @@
     </row>
     <row r="6" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>67</v>
@@ -4885,7 +4875,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>67</v>

</xml_diff>